<commit_message>
Fire 07, 07_2, 08, 08_2 추가
</commit_message>
<xml_diff>
--- a/기획서/맵 배치도.xlsx
+++ b/기획서/맵 배치도.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seongjae Yoon\Desktop\MonsterHunterSoldier\Kronos2\기획서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\윤성재\Desktop\Kronos\Kronos2\기획서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{159869B7-3433-4744-8D72-8AFDD526FEFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7E95DF-5FD3-4FA3-843B-6CA4BF810378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="0" windowWidth="19275" windowHeight="15600" xr2:uid="{6D85DBDB-473E-4678-882C-F5AC79603B82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D85DBDB-473E-4678-882C-F5AC79603B82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>테마</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,10 +61,6 @@
   </si>
   <si>
     <t>식물</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>식당</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -519,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CABBE2-8A83-496E-B32E-B5FE05215AB9}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -539,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2">
         <v>1</v>
@@ -593,45 +589,45 @@
         <v>17</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V2" s="2">
         <f>B2-COUNTA(C2:U2)</f>
@@ -646,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" ref="V3:V9" si="0">B3-COUNTA(C3:U3)</f>
@@ -661,10 +657,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="0"/>
@@ -679,10 +675,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" si="0"/>
@@ -697,10 +693,10 @@
         <v>2</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V6" s="2">
         <f t="shared" si="0"/>
@@ -715,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V7" s="2">
         <f t="shared" si="0"/>
@@ -727,30 +723,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="V8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>